<commit_message>
Updated DataSet, fixed Dead Kernel Problem, sped up the proccess and completed the first order approximation test. Only one more left
</commit_message>
<xml_diff>
--- a/sampleDataSet.xlsx
+++ b/sampleDataSet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gilpasternak/Downloads/Likelihood/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ADD9563B-A6A2-F143-BB2A-81C0F3C1895F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349190F8-DC65-3D4F-A1E2-51EEC342EF13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16620" xr2:uid="{1F8DA360-E974-914A-BB29-6C10CB151BF2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="20">
   <si>
     <t>Email</t>
   </si>
@@ -85,6 +85,15 @@
   <si>
     <t>San Digo. CA</t>
   </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weight </t>
+  </si>
 </sst>
 </file>
 
@@ -135,11 +144,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -455,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22315E7-23A9-A543-A0A9-36943FB40866}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:F123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -468,7 +478,7 @@
     <col min="3" max="3" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -478,8 +488,22 @@
       <c r="C1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -489,8 +513,17 @@
       <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>70</v>
+      </c>
+      <c r="E3">
+        <v>45000</v>
+      </c>
+      <c r="F3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -500,8 +533,17 @@
       <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>71</v>
+      </c>
+      <c r="E4">
+        <v>50000</v>
+      </c>
+      <c r="F4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -511,8 +553,17 @@
       <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>72</v>
+      </c>
+      <c r="E5">
+        <v>55000</v>
+      </c>
+      <c r="F5">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -522,8 +573,17 @@
       <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>73</v>
+      </c>
+      <c r="E6">
+        <v>60000</v>
+      </c>
+      <c r="F6">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -533,8 +593,17 @@
       <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>74</v>
+      </c>
+      <c r="E7">
+        <v>45000</v>
+      </c>
+      <c r="F7">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
@@ -544,8 +613,17 @@
       <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>75</v>
+      </c>
+      <c r="E8">
+        <v>50000</v>
+      </c>
+      <c r="F8">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -555,8 +633,17 @@
       <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>76</v>
+      </c>
+      <c r="E9">
+        <v>55000</v>
+      </c>
+      <c r="F9">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -566,8 +653,17 @@
       <c r="C10" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>77</v>
+      </c>
+      <c r="E10">
+        <v>60000</v>
+      </c>
+      <c r="F10">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -577,8 +673,17 @@
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>64</v>
+      </c>
+      <c r="E11">
+        <v>45000</v>
+      </c>
+      <c r="F11">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -588,8 +693,17 @@
       <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>61</v>
+      </c>
+      <c r="E12">
+        <v>50000</v>
+      </c>
+      <c r="F12">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
@@ -599,8 +713,17 @@
       <c r="C13" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>58</v>
+      </c>
+      <c r="E13">
+        <v>55000</v>
+      </c>
+      <c r="F13">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -610,8 +733,17 @@
       <c r="C14" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <v>55</v>
+      </c>
+      <c r="E14">
+        <v>60000</v>
+      </c>
+      <c r="F14">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -621,8 +753,17 @@
       <c r="C15" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>52</v>
+      </c>
+      <c r="E15">
+        <v>45000</v>
+      </c>
+      <c r="F15">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
@@ -632,8 +773,17 @@
       <c r="C16" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>63</v>
+      </c>
+      <c r="E16">
+        <v>50000</v>
+      </c>
+      <c r="F16">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
@@ -643,8 +793,17 @@
       <c r="C17" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>62.4</v>
+      </c>
+      <c r="E17">
+        <v>55000</v>
+      </c>
+      <c r="F17">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>1</v>
       </c>
@@ -654,8 +813,17 @@
       <c r="C18" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <v>62.7</v>
+      </c>
+      <c r="E18">
+        <v>60000</v>
+      </c>
+      <c r="F18">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
@@ -665,8 +833,17 @@
       <c r="C19" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <v>62.4</v>
+      </c>
+      <c r="E19">
+        <v>45000</v>
+      </c>
+      <c r="F19">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
@@ -676,8 +853,17 @@
       <c r="C20" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <v>62.25</v>
+      </c>
+      <c r="E20">
+        <v>50000</v>
+      </c>
+      <c r="F20">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
@@ -687,8 +873,17 @@
       <c r="C21" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <v>62.1</v>
+      </c>
+      <c r="E21">
+        <v>55000</v>
+      </c>
+      <c r="F21">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>5</v>
       </c>
@@ -698,8 +893,17 @@
       <c r="C22" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <v>61.95</v>
+      </c>
+      <c r="E22">
+        <v>60000</v>
+      </c>
+      <c r="F22">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>1</v>
       </c>
@@ -709,8 +913,17 @@
       <c r="C23" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <v>61.8</v>
+      </c>
+      <c r="E23">
+        <v>45000</v>
+      </c>
+      <c r="F23">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
@@ -720,8 +933,17 @@
       <c r="C24" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <v>72</v>
+      </c>
+      <c r="E24">
+        <v>50000</v>
+      </c>
+      <c r="F24">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
@@ -731,8 +953,17 @@
       <c r="C25" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <v>79</v>
+      </c>
+      <c r="E25">
+        <v>55000</v>
+      </c>
+      <c r="F25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>4</v>
       </c>
@@ -742,8 +973,17 @@
       <c r="C26" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <v>71</v>
+      </c>
+      <c r="E26">
+        <v>60000</v>
+      </c>
+      <c r="F26">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>5</v>
       </c>
@@ -753,8 +993,17 @@
       <c r="C27" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27">
+        <v>75</v>
+      </c>
+      <c r="E27">
+        <v>45000</v>
+      </c>
+      <c r="F27">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
@@ -764,8 +1013,17 @@
       <c r="C28" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28">
+        <v>74.5</v>
+      </c>
+      <c r="E28">
+        <v>50000</v>
+      </c>
+      <c r="F28">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>1</v>
       </c>
@@ -775,8 +1033,17 @@
       <c r="C29" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="E29">
+        <v>55000</v>
+      </c>
+      <c r="F29">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>2</v>
       </c>
@@ -786,8 +1053,17 @@
       <c r="C30" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30">
+        <v>74.7</v>
+      </c>
+      <c r="E30">
+        <v>60000</v>
+      </c>
+      <c r="F30">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
@@ -797,8 +1073,17 @@
       <c r="C31" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31">
+        <v>64</v>
+      </c>
+      <c r="E31">
+        <v>45000</v>
+      </c>
+      <c r="F31">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>4</v>
       </c>
@@ -808,8 +1093,17 @@
       <c r="C32" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <v>65</v>
+      </c>
+      <c r="E32">
+        <v>50000</v>
+      </c>
+      <c r="F32">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>5</v>
       </c>
@@ -819,8 +1113,17 @@
       <c r="C33" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33">
+        <v>66</v>
+      </c>
+      <c r="E33">
+        <v>55000</v>
+      </c>
+      <c r="F33">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -830,8 +1133,17 @@
       <c r="C34" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34">
+        <v>67</v>
+      </c>
+      <c r="E34">
+        <v>60000</v>
+      </c>
+      <c r="F34">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>1</v>
       </c>
@@ -841,8 +1153,17 @@
       <c r="C35" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35">
+        <v>68</v>
+      </c>
+      <c r="E35">
+        <v>45000</v>
+      </c>
+      <c r="F35">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>2</v>
       </c>
@@ -852,8 +1173,17 @@
       <c r="C36" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36">
+        <v>69</v>
+      </c>
+      <c r="E36">
+        <v>50000</v>
+      </c>
+      <c r="F36">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>3</v>
       </c>
@@ -863,8 +1193,17 @@
       <c r="C37" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37">
+        <v>70</v>
+      </c>
+      <c r="E37">
+        <v>55000</v>
+      </c>
+      <c r="F37">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>4</v>
       </c>
@@ -874,8 +1213,17 @@
       <c r="C38" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38">
+        <v>71</v>
+      </c>
+      <c r="E38">
+        <v>60000</v>
+      </c>
+      <c r="F38">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>5</v>
       </c>
@@ -885,8 +1233,17 @@
       <c r="C39" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39">
+        <v>72</v>
+      </c>
+      <c r="E39">
+        <v>45000</v>
+      </c>
+      <c r="F39" s="4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>5</v>
       </c>
@@ -896,8 +1253,17 @@
       <c r="C40" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40">
+        <v>73</v>
+      </c>
+      <c r="E40">
+        <v>50000</v>
+      </c>
+      <c r="F40" s="4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>5</v>
       </c>
@@ -907,9 +1273,1652 @@
       <c r="C41" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C42" s="3"/>
+      <c r="D41">
+        <v>74</v>
+      </c>
+      <c r="E41">
+        <v>55000</v>
+      </c>
+      <c r="F41" s="4">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42">
+        <v>52</v>
+      </c>
+      <c r="E42">
+        <v>60000</v>
+      </c>
+      <c r="F42" s="4">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43">
+        <v>63</v>
+      </c>
+      <c r="E43">
+        <v>45000</v>
+      </c>
+      <c r="F43" s="4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44">
+        <v>62.4</v>
+      </c>
+      <c r="E44">
+        <v>50000</v>
+      </c>
+      <c r="F44" s="4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45">
+        <v>62.7</v>
+      </c>
+      <c r="E45">
+        <v>55000</v>
+      </c>
+      <c r="F45" s="4">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46">
+        <v>62.4</v>
+      </c>
+      <c r="E46">
+        <v>60000</v>
+      </c>
+      <c r="F46" s="4">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47">
+        <v>62.25</v>
+      </c>
+      <c r="E47">
+        <v>45000</v>
+      </c>
+      <c r="F47" s="4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48">
+        <v>62.1</v>
+      </c>
+      <c r="E48">
+        <v>50000</v>
+      </c>
+      <c r="F48" s="4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49">
+        <v>61.95</v>
+      </c>
+      <c r="E49">
+        <v>55000</v>
+      </c>
+      <c r="F49" s="4">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50">
+        <v>61.8</v>
+      </c>
+      <c r="E50">
+        <v>60000</v>
+      </c>
+      <c r="F50" s="4">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51">
+        <v>72</v>
+      </c>
+      <c r="E51">
+        <v>4500</v>
+      </c>
+      <c r="F51" s="4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52">
+        <v>79</v>
+      </c>
+      <c r="F52" s="4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53">
+        <v>71</v>
+      </c>
+      <c r="E53">
+        <v>850850043</v>
+      </c>
+      <c r="F53" s="4">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54">
+        <v>70</v>
+      </c>
+      <c r="E54">
+        <v>45000</v>
+      </c>
+      <c r="F54">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55">
+        <v>71</v>
+      </c>
+      <c r="E55">
+        <v>50000</v>
+      </c>
+      <c r="F55">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B56" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56">
+        <v>72</v>
+      </c>
+      <c r="E56">
+        <v>55000</v>
+      </c>
+      <c r="F56">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B57" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57">
+        <v>73</v>
+      </c>
+      <c r="E57">
+        <v>60000</v>
+      </c>
+      <c r="F57">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58">
+        <v>74</v>
+      </c>
+      <c r="E58">
+        <v>45000</v>
+      </c>
+      <c r="F58">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59">
+        <v>75</v>
+      </c>
+      <c r="E59">
+        <v>50000</v>
+      </c>
+      <c r="F59">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B60" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60">
+        <v>76</v>
+      </c>
+      <c r="E60">
+        <v>55000</v>
+      </c>
+      <c r="F60">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B61" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61">
+        <v>77</v>
+      </c>
+      <c r="E61">
+        <v>60000</v>
+      </c>
+      <c r="F61">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D62">
+        <v>64</v>
+      </c>
+      <c r="E62">
+        <v>45000</v>
+      </c>
+      <c r="F62">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D63">
+        <v>61</v>
+      </c>
+      <c r="E63">
+        <v>50000</v>
+      </c>
+      <c r="F63">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B64" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64">
+        <v>70</v>
+      </c>
+      <c r="E64">
+        <v>45000</v>
+      </c>
+      <c r="F64">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B65" t="s">
+        <v>9</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65">
+        <v>71</v>
+      </c>
+      <c r="E65">
+        <v>50000</v>
+      </c>
+      <c r="F65">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66">
+        <v>72</v>
+      </c>
+      <c r="E66">
+        <v>55000</v>
+      </c>
+      <c r="F66">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B67" t="s">
+        <v>11</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67">
+        <v>73</v>
+      </c>
+      <c r="E67">
+        <v>60000</v>
+      </c>
+      <c r="F67">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68" t="s">
+        <v>8</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D68">
+        <v>74</v>
+      </c>
+      <c r="E68">
+        <v>45000</v>
+      </c>
+      <c r="F68">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B69" t="s">
+        <v>9</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69">
+        <v>75</v>
+      </c>
+      <c r="E69">
+        <v>50000</v>
+      </c>
+      <c r="F69">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70" t="s">
+        <v>10</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70">
+        <v>76</v>
+      </c>
+      <c r="E70">
+        <v>55000</v>
+      </c>
+      <c r="F70">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B71" t="s">
+        <v>11</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D71">
+        <v>77</v>
+      </c>
+      <c r="E71">
+        <v>60000</v>
+      </c>
+      <c r="F71">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B72" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D72">
+        <v>64</v>
+      </c>
+      <c r="E72">
+        <v>45000</v>
+      </c>
+      <c r="F72">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73" t="s">
+        <v>9</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D73">
+        <v>61</v>
+      </c>
+      <c r="E73">
+        <v>50000</v>
+      </c>
+      <c r="F73">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B74" t="s">
+        <v>8</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D74">
+        <v>70</v>
+      </c>
+      <c r="E74">
+        <v>45000</v>
+      </c>
+      <c r="F74">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B75" t="s">
+        <v>9</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D75">
+        <v>71</v>
+      </c>
+      <c r="E75">
+        <v>50000</v>
+      </c>
+      <c r="F75">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B76" t="s">
+        <v>10</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D76">
+        <v>72</v>
+      </c>
+      <c r="E76">
+        <v>55000</v>
+      </c>
+      <c r="F76">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B77" t="s">
+        <v>11</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D77">
+        <v>73</v>
+      </c>
+      <c r="E77">
+        <v>60000</v>
+      </c>
+      <c r="F77">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B78" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D78">
+        <v>74</v>
+      </c>
+      <c r="E78">
+        <v>45000</v>
+      </c>
+      <c r="F78">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B79" t="s">
+        <v>9</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D79">
+        <v>75</v>
+      </c>
+      <c r="E79">
+        <v>50000</v>
+      </c>
+      <c r="F79">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B80" t="s">
+        <v>10</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D80">
+        <v>76</v>
+      </c>
+      <c r="E80">
+        <v>55000</v>
+      </c>
+      <c r="F80">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B81" t="s">
+        <v>11</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D81">
+        <v>77</v>
+      </c>
+      <c r="E81">
+        <v>60000</v>
+      </c>
+      <c r="F81">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B82" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D82">
+        <v>64</v>
+      </c>
+      <c r="E82">
+        <v>45000</v>
+      </c>
+      <c r="F82">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B83" t="s">
+        <v>9</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D83">
+        <v>61</v>
+      </c>
+      <c r="E83">
+        <v>50000</v>
+      </c>
+      <c r="F83">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B84" t="s">
+        <v>8</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D84">
+        <v>70</v>
+      </c>
+      <c r="E84">
+        <v>45000</v>
+      </c>
+      <c r="F84">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B85" t="s">
+        <v>9</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D85">
+        <v>71</v>
+      </c>
+      <c r="E85">
+        <v>50000</v>
+      </c>
+      <c r="F85">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B86" t="s">
+        <v>10</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D86">
+        <v>72</v>
+      </c>
+      <c r="E86">
+        <v>55000</v>
+      </c>
+      <c r="F86">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B87" t="s">
+        <v>11</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D87">
+        <v>73</v>
+      </c>
+      <c r="E87">
+        <v>60000</v>
+      </c>
+      <c r="F87">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B88" t="s">
+        <v>8</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D88">
+        <v>74</v>
+      </c>
+      <c r="E88">
+        <v>45000</v>
+      </c>
+      <c r="F88">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B89" t="s">
+        <v>9</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D89">
+        <v>75</v>
+      </c>
+      <c r="E89">
+        <v>50000</v>
+      </c>
+      <c r="F89">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B90" t="s">
+        <v>10</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D90">
+        <v>76</v>
+      </c>
+      <c r="E90">
+        <v>55000</v>
+      </c>
+      <c r="F90">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B91" t="s">
+        <v>11</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D91">
+        <v>77</v>
+      </c>
+      <c r="E91">
+        <v>60000</v>
+      </c>
+      <c r="F91">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B92" t="s">
+        <v>8</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D92">
+        <v>64</v>
+      </c>
+      <c r="E92">
+        <v>45000</v>
+      </c>
+      <c r="F92">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B93" t="s">
+        <v>9</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D93">
+        <v>61</v>
+      </c>
+      <c r="E93">
+        <v>50000</v>
+      </c>
+      <c r="F93">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B94" t="s">
+        <v>8</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D94">
+        <v>70</v>
+      </c>
+      <c r="E94">
+        <v>45000</v>
+      </c>
+      <c r="F94">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B95" t="s">
+        <v>9</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D95">
+        <v>71</v>
+      </c>
+      <c r="E95">
+        <v>50000</v>
+      </c>
+      <c r="F95">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B96" t="s">
+        <v>10</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D96">
+        <v>72</v>
+      </c>
+      <c r="E96">
+        <v>55000</v>
+      </c>
+      <c r="F96">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B97" t="s">
+        <v>11</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D97">
+        <v>73</v>
+      </c>
+      <c r="E97">
+        <v>60000</v>
+      </c>
+      <c r="F97">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B98" t="s">
+        <v>8</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D98">
+        <v>74</v>
+      </c>
+      <c r="E98">
+        <v>45000</v>
+      </c>
+      <c r="F98">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B99" t="s">
+        <v>9</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D99">
+        <v>75</v>
+      </c>
+      <c r="E99">
+        <v>50000</v>
+      </c>
+      <c r="F99">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B100" t="s">
+        <v>10</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D100">
+        <v>76</v>
+      </c>
+      <c r="E100">
+        <v>55000</v>
+      </c>
+      <c r="F100">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B101" t="s">
+        <v>11</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D101">
+        <v>77</v>
+      </c>
+      <c r="E101">
+        <v>60000</v>
+      </c>
+      <c r="F101">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B102" t="s">
+        <v>8</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D102">
+        <v>64</v>
+      </c>
+      <c r="E102">
+        <v>45000</v>
+      </c>
+      <c r="F102">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B103" t="s">
+        <v>9</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D103">
+        <v>61</v>
+      </c>
+      <c r="E103">
+        <v>50000</v>
+      </c>
+      <c r="F103">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B104" t="s">
+        <v>8</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D104">
+        <v>70</v>
+      </c>
+      <c r="E104">
+        <v>45000</v>
+      </c>
+      <c r="F104">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B105" t="s">
+        <v>9</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D105">
+        <v>71</v>
+      </c>
+      <c r="E105">
+        <v>50000</v>
+      </c>
+      <c r="F105">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A106" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B106" t="s">
+        <v>10</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D106">
+        <v>72</v>
+      </c>
+      <c r="E106">
+        <v>55000</v>
+      </c>
+      <c r="F106">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A107" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B107" t="s">
+        <v>11</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D107">
+        <v>73</v>
+      </c>
+      <c r="E107">
+        <v>60000</v>
+      </c>
+      <c r="F107">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A108" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B108" t="s">
+        <v>8</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D108">
+        <v>74</v>
+      </c>
+      <c r="E108">
+        <v>45000</v>
+      </c>
+      <c r="F108">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A109" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B109" t="s">
+        <v>9</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D109">
+        <v>75</v>
+      </c>
+      <c r="E109">
+        <v>50000</v>
+      </c>
+      <c r="F109">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A110" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B110" t="s">
+        <v>10</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D110">
+        <v>76</v>
+      </c>
+      <c r="E110">
+        <v>55000</v>
+      </c>
+      <c r="F110">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A111" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B111" t="s">
+        <v>11</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D111">
+        <v>77</v>
+      </c>
+      <c r="E111">
+        <v>60000</v>
+      </c>
+      <c r="F111">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A112" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B112" t="s">
+        <v>8</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D112">
+        <v>64</v>
+      </c>
+      <c r="E112">
+        <v>45000</v>
+      </c>
+      <c r="F112">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A113" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B113" t="s">
+        <v>9</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D113">
+        <v>61</v>
+      </c>
+      <c r="E113">
+        <v>50000</v>
+      </c>
+      <c r="F113">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A114" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B114" t="s">
+        <v>8</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D114">
+        <v>70</v>
+      </c>
+      <c r="E114">
+        <v>45000</v>
+      </c>
+      <c r="F114">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A115" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B115" t="s">
+        <v>9</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D115">
+        <v>71</v>
+      </c>
+      <c r="E115">
+        <v>50000</v>
+      </c>
+      <c r="F115">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A116" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B116" t="s">
+        <v>10</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D116">
+        <v>72</v>
+      </c>
+      <c r="E116">
+        <v>55000</v>
+      </c>
+      <c r="F116">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A117" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B117" t="s">
+        <v>11</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D117">
+        <v>73</v>
+      </c>
+      <c r="E117">
+        <v>60000</v>
+      </c>
+      <c r="F117">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A118" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B118" t="s">
+        <v>8</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D118">
+        <v>74</v>
+      </c>
+      <c r="E118">
+        <v>45000</v>
+      </c>
+      <c r="F118">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A119" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B119" t="s">
+        <v>9</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D119">
+        <v>75</v>
+      </c>
+      <c r="E119">
+        <v>50000</v>
+      </c>
+      <c r="F119">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A120" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B120" t="s">
+        <v>10</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D120">
+        <v>76</v>
+      </c>
+      <c r="E120">
+        <v>55000</v>
+      </c>
+      <c r="F120">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A121" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B121" t="s">
+        <v>11</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D121">
+        <v>77</v>
+      </c>
+      <c r="E121">
+        <v>60000</v>
+      </c>
+      <c r="F121">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A122" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B122" t="s">
+        <v>8</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D122">
+        <v>64</v>
+      </c>
+      <c r="E122">
+        <v>45000</v>
+      </c>
+      <c r="F122">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A123" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B123" t="s">
+        <v>9</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D123">
+        <v>61</v>
+      </c>
+      <c r="E123">
+        <v>50000</v>
+      </c>
+      <c r="F123">
+        <v>180</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -950,6 +2959,88 @@
     <hyperlink ref="A38" r:id="rId35" xr:uid="{85A4BF0C-733E-824C-9D97-F90369383D0E}"/>
     <hyperlink ref="A39" r:id="rId36" xr:uid="{C58DA7E5-76D5-234C-893D-3C22D73B2586}"/>
     <hyperlink ref="A41" r:id="rId37" xr:uid="{7AE08EA5-880A-C647-A2C4-DF717C31AF9F}"/>
+    <hyperlink ref="A42" r:id="rId38" xr:uid="{66054D11-BC7E-5647-90D5-F427EC3F8F51}"/>
+    <hyperlink ref="A43" r:id="rId39" xr:uid="{327E1A36-4759-7C41-9D2A-74D709FFE304}"/>
+    <hyperlink ref="A44" r:id="rId40" xr:uid="{AC57D2AD-E90F-2A49-A78D-7DB6E6BF519B}"/>
+    <hyperlink ref="A45" r:id="rId41" xr:uid="{0DC5FFEA-3B6D-144E-9CC6-148C77429102}"/>
+    <hyperlink ref="A46" r:id="rId42" xr:uid="{63E6F276-EDDA-A346-B774-D568C22A4E01}"/>
+    <hyperlink ref="A47" r:id="rId43" xr:uid="{B8765458-C34B-184C-9EC2-D09C09F4B8FF}"/>
+    <hyperlink ref="A48" r:id="rId44" xr:uid="{7C4BEA35-E464-F74E-9FA2-88184BD8ECC8}"/>
+    <hyperlink ref="A49" r:id="rId45" xr:uid="{71A68FAC-CD8F-DD42-9A9D-0D3149810D72}"/>
+    <hyperlink ref="A50" r:id="rId46" xr:uid="{3AADC7D9-C674-EE40-BE92-24767DCCE669}"/>
+    <hyperlink ref="A51" r:id="rId47" xr:uid="{B1FE661A-3535-4D45-B127-51EB088B3CA1}"/>
+    <hyperlink ref="A52" r:id="rId48" xr:uid="{CE0B881F-F29D-2244-B6D3-FE584C58F310}"/>
+    <hyperlink ref="A53" r:id="rId49" xr:uid="{A1FA0DAE-192B-2649-9527-315B2973ECF5}"/>
+    <hyperlink ref="A54" r:id="rId50" xr:uid="{AB9DC471-9B12-7344-97EA-47DFFAEAE26D}"/>
+    <hyperlink ref="A55" r:id="rId51" xr:uid="{75F659B4-2B9B-5E4F-8338-B7EA6CE562BC}"/>
+    <hyperlink ref="A56" r:id="rId52" xr:uid="{28179641-E9B5-AC4C-9F65-5B3EDF612C99}"/>
+    <hyperlink ref="A57" r:id="rId53" xr:uid="{48ECC313-E51E-1847-9301-6108E33460B5}"/>
+    <hyperlink ref="A58" r:id="rId54" xr:uid="{57D3F186-8145-D041-BC64-51A02AE45FCE}"/>
+    <hyperlink ref="A59" r:id="rId55" xr:uid="{BD681423-71EB-0941-9B3E-6B5BE5225E1E}"/>
+    <hyperlink ref="A60" r:id="rId56" xr:uid="{38D73760-4AAE-184A-8366-D8312512D0D5}"/>
+    <hyperlink ref="A61" r:id="rId57" xr:uid="{5897EF63-F62B-5645-9590-C26FEF0FD53B}"/>
+    <hyperlink ref="A62" r:id="rId58" xr:uid="{4C8395E6-9F07-514F-91E2-38020FC0CC7E}"/>
+    <hyperlink ref="A63" r:id="rId59" xr:uid="{EA0351CF-4AD7-1F49-BB63-8CC91C36C58B}"/>
+    <hyperlink ref="A64" r:id="rId60" xr:uid="{B4ECF38E-7498-7146-9D71-8B347CBE2700}"/>
+    <hyperlink ref="A65" r:id="rId61" xr:uid="{BE2CBC52-C449-9842-A6F1-014BFAFFAF44}"/>
+    <hyperlink ref="A66" r:id="rId62" xr:uid="{7ABBF4D9-FF0D-9445-B423-588781194B8D}"/>
+    <hyperlink ref="A67" r:id="rId63" xr:uid="{9C4720A1-F05E-2D4C-A749-843D73696487}"/>
+    <hyperlink ref="A68" r:id="rId64" xr:uid="{E45F331A-92EF-0646-87C6-8D6079264E30}"/>
+    <hyperlink ref="A69" r:id="rId65" xr:uid="{01898390-EE2F-674B-80D0-30C50485B8AA}"/>
+    <hyperlink ref="A70" r:id="rId66" xr:uid="{FE71FA25-429A-174B-AE5F-39B2F8414389}"/>
+    <hyperlink ref="A71" r:id="rId67" xr:uid="{9FFEA32A-8915-D94C-8D7B-15DBE1DB6E65}"/>
+    <hyperlink ref="A72" r:id="rId68" xr:uid="{01BC8C4B-7946-FA44-B094-96118D8E606E}"/>
+    <hyperlink ref="A73" r:id="rId69" xr:uid="{B6C9937D-341F-C84A-9617-3B75BE6BDF83}"/>
+    <hyperlink ref="A74" r:id="rId70" xr:uid="{A55E60CA-8425-5D41-AA41-E9DEDBBE9CAA}"/>
+    <hyperlink ref="A75" r:id="rId71" xr:uid="{4C4DA813-D5A1-3F45-84FA-5219ACFD37CF}"/>
+    <hyperlink ref="A76" r:id="rId72" xr:uid="{3CD7632E-6DAF-1F4F-9928-EEC7534EE860}"/>
+    <hyperlink ref="A77" r:id="rId73" xr:uid="{353F601D-3D2D-3740-920C-0165A207AAB7}"/>
+    <hyperlink ref="A78" r:id="rId74" xr:uid="{F78F6281-2BB6-334A-8528-C225781F6552}"/>
+    <hyperlink ref="A79" r:id="rId75" xr:uid="{6EA69795-E68C-C843-ABF9-CB7B935962D3}"/>
+    <hyperlink ref="A80" r:id="rId76" xr:uid="{C5B031DB-6133-E145-B7B6-50025F3CB312}"/>
+    <hyperlink ref="A81" r:id="rId77" xr:uid="{19A06DDC-4A4B-E147-B185-A30F3652E30C}"/>
+    <hyperlink ref="A82" r:id="rId78" xr:uid="{D7C9F70F-BB60-DA48-8A4E-1585E13DF06F}"/>
+    <hyperlink ref="A83" r:id="rId79" xr:uid="{ACAB2302-AF58-EB4C-81FE-E17F974CC398}"/>
+    <hyperlink ref="A84" r:id="rId80" xr:uid="{17B861AD-53BC-3342-9E7B-EB2311B1EE3A}"/>
+    <hyperlink ref="A85" r:id="rId81" xr:uid="{75C133E8-F37F-7144-BC43-DE3BC18B40DA}"/>
+    <hyperlink ref="A86" r:id="rId82" xr:uid="{273262E6-B137-B94C-A276-A9E25FB07285}"/>
+    <hyperlink ref="A87" r:id="rId83" xr:uid="{14F344AC-B69F-364A-964E-8FDDBD9713D7}"/>
+    <hyperlink ref="A88" r:id="rId84" xr:uid="{73339963-DA30-B747-93CF-8D6A8632CF23}"/>
+    <hyperlink ref="A89" r:id="rId85" xr:uid="{016E231B-B42E-8042-A450-F140AD909AA3}"/>
+    <hyperlink ref="A90" r:id="rId86" xr:uid="{AB0EADD8-318D-1942-9F42-A5E69DAFA011}"/>
+    <hyperlink ref="A91" r:id="rId87" xr:uid="{74B8EB11-1FEC-DB48-A5E8-9FEFA01455DF}"/>
+    <hyperlink ref="A92" r:id="rId88" xr:uid="{184B35D2-2EE0-1E46-A8D1-CC7AC53C8346}"/>
+    <hyperlink ref="A93" r:id="rId89" xr:uid="{38DBCCED-80B5-7748-B84C-B3B1EA3C36A9}"/>
+    <hyperlink ref="A94" r:id="rId90" xr:uid="{574B36C2-20B6-CF45-9FA3-BD58DBE7DD5C}"/>
+    <hyperlink ref="A95" r:id="rId91" xr:uid="{C99B7BB3-D339-A147-859E-082FFD822BF9}"/>
+    <hyperlink ref="A96" r:id="rId92" xr:uid="{46CF7CDF-A7D8-AF42-8F0F-783054542CF6}"/>
+    <hyperlink ref="A97" r:id="rId93" xr:uid="{CE316EDF-784D-E848-878D-22E1DDBB9B3D}"/>
+    <hyperlink ref="A98" r:id="rId94" xr:uid="{C47A0690-71B2-444F-9D0D-F446A20CC071}"/>
+    <hyperlink ref="A99" r:id="rId95" xr:uid="{C034871B-8229-244F-B14F-C05397FB3CD0}"/>
+    <hyperlink ref="A100" r:id="rId96" xr:uid="{54F6DA0E-010E-764E-B302-3CB213CC92CB}"/>
+    <hyperlink ref="A101" r:id="rId97" xr:uid="{AAD36A97-A565-1D42-B1A7-8D16B67B64C1}"/>
+    <hyperlink ref="A102" r:id="rId98" xr:uid="{D91530EA-31C4-134C-B54F-BDDDBCF78262}"/>
+    <hyperlink ref="A103" r:id="rId99" xr:uid="{507897DC-4DB7-264A-8927-F281ADB42490}"/>
+    <hyperlink ref="A104" r:id="rId100" xr:uid="{06039A28-A3E3-FC47-A6F4-54E13BFF5881}"/>
+    <hyperlink ref="A105" r:id="rId101" xr:uid="{8CF8B506-A2C2-B147-83D3-01E36A02F487}"/>
+    <hyperlink ref="A106" r:id="rId102" xr:uid="{37DB3637-52AA-A34D-97F6-A490FBAFEC95}"/>
+    <hyperlink ref="A107" r:id="rId103" xr:uid="{B6D5D36B-8AE3-A643-BFBB-9D854D2588EA}"/>
+    <hyperlink ref="A108" r:id="rId104" xr:uid="{C05E606C-FD2F-4A4E-A96E-602EAE28A2BF}"/>
+    <hyperlink ref="A109" r:id="rId105" xr:uid="{BE4566D6-EA92-6449-85B8-9C3391D749A7}"/>
+    <hyperlink ref="A110" r:id="rId106" xr:uid="{2A0639E6-B8EA-8A4C-A491-C05676EDF598}"/>
+    <hyperlink ref="A111" r:id="rId107" xr:uid="{0D5CF662-4D17-E349-A885-FAD30B3F3F25}"/>
+    <hyperlink ref="A112" r:id="rId108" xr:uid="{F2606543-3464-014C-B1E2-ABA9D3E1167C}"/>
+    <hyperlink ref="A113" r:id="rId109" xr:uid="{FABCB166-920D-2341-B1D5-025CE5FBC213}"/>
+    <hyperlink ref="A114" r:id="rId110" xr:uid="{528E7B08-CBF7-ED4F-A94A-6C51766409E3}"/>
+    <hyperlink ref="A115" r:id="rId111" xr:uid="{C55933B2-0F74-6146-8036-81EAF945F001}"/>
+    <hyperlink ref="A116" r:id="rId112" xr:uid="{C14B41C0-BF7A-1843-AE9A-E33B9BA88296}"/>
+    <hyperlink ref="A117" r:id="rId113" xr:uid="{AA047EAC-DF4E-F348-8303-3AA9EEF792D7}"/>
+    <hyperlink ref="A118" r:id="rId114" xr:uid="{EFE22E7E-DADD-A947-9173-14F20DFDE6D9}"/>
+    <hyperlink ref="A119" r:id="rId115" xr:uid="{B350091F-F59D-BD49-AD0D-0F3FC7FAE347}"/>
+    <hyperlink ref="A120" r:id="rId116" xr:uid="{1521FF04-1AD1-AC46-9470-FE4E0E68102F}"/>
+    <hyperlink ref="A121" r:id="rId117" xr:uid="{59F0C557-64B0-2045-9226-0761F48DB1B4}"/>
+    <hyperlink ref="A122" r:id="rId118" xr:uid="{189D99BE-4F95-D24E-B6B2-F3123876AC5E}"/>
+    <hyperlink ref="A123" r:id="rId119" xr:uid="{34C8C161-8D39-6843-BDB3-F17DFCEFB540}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
TimeSeries and Kernel fully production ready, PCA, Categoricals and report left to go
</commit_message>
<xml_diff>
--- a/sampleDataSet.xlsx
+++ b/sampleDataSet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gilpasternak/Downloads/Likelihood/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349190F8-DC65-3D4F-A1E2-51EEC342EF13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF1197A-3DAB-CA48-B047-33E6DDAA3D2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16620" xr2:uid="{1F8DA360-E974-914A-BB29-6C10CB151BF2}"/>
   </bookViews>
@@ -92,7 +92,7 @@
     <t>Salary</t>
   </si>
   <si>
-    <t xml:space="preserve">Weight </t>
+    <t>Weight</t>
   </si>
 </sst>
 </file>
@@ -467,9 +467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22315E7-23A9-A543-A0A9-36943FB40866}">
   <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Synthetic dataset made larger, PCA class fully functional, weird Kernel-PCA issue
</commit_message>
<xml_diff>
--- a/sampleDataSet.xlsx
+++ b/sampleDataSet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gilpasternak/Downloads/Likelihood/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF1197A-3DAB-CA48-B047-33E6DDAA3D2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC2BBBD-3D58-3E47-ADB4-566C733E060C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16620" xr2:uid="{1F8DA360-E974-914A-BB29-6C10CB151BF2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="22">
   <si>
     <t>Email</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>Weight</t>
+  </si>
+  <si>
+    <t>ellen@gmail.com</t>
+  </si>
+  <si>
+    <t>Gil@syntheticData**</t>
   </si>
 </sst>
 </file>
@@ -465,9 +471,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22315E7-23A9-A543-A0A9-36943FB40866}">
-  <dimension ref="A1:F123"/>
+  <dimension ref="A1:F159"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="F134" sqref="F134"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -497,8 +505,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="D2">
         <v>80</v>
+      </c>
+      <c r="F2">
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2915,6 +2929,726 @@
         <v>50000</v>
       </c>
       <c r="F123">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A124" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B124" t="s">
+        <v>10</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D124">
+        <v>76</v>
+      </c>
+      <c r="E124">
+        <v>55000</v>
+      </c>
+      <c r="F124">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A125" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B125" t="s">
+        <v>11</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D125">
+        <v>77</v>
+      </c>
+      <c r="E125">
+        <v>60000</v>
+      </c>
+      <c r="F125">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A126" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B126" t="s">
+        <v>8</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D126">
+        <v>64</v>
+      </c>
+      <c r="E126">
+        <v>45000</v>
+      </c>
+      <c r="F126">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A127" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B127" t="s">
+        <v>9</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D127">
+        <v>61</v>
+      </c>
+      <c r="E127">
+        <v>50000</v>
+      </c>
+      <c r="F127">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A128" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B128" t="s">
+        <v>10</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D128">
+        <v>76</v>
+      </c>
+      <c r="E128">
+        <v>55000</v>
+      </c>
+      <c r="F128">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A129" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B129" t="s">
+        <v>11</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D129">
+        <v>77</v>
+      </c>
+      <c r="E129">
+        <v>60000</v>
+      </c>
+      <c r="F129">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A130" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B130" t="s">
+        <v>8</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D130">
+        <v>64</v>
+      </c>
+      <c r="E130">
+        <v>45000</v>
+      </c>
+      <c r="F130">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A131" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B131" t="s">
+        <v>9</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D131">
+        <v>61</v>
+      </c>
+      <c r="E131">
+        <v>50000</v>
+      </c>
+      <c r="F131">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A132" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B132" t="s">
+        <v>10</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D132">
+        <v>76</v>
+      </c>
+      <c r="E132">
+        <v>55000</v>
+      </c>
+      <c r="F132">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A133" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B133" t="b">
+        <v>0</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D133">
+        <v>77</v>
+      </c>
+      <c r="E133">
+        <v>60000</v>
+      </c>
+      <c r="F133">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A134" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B134" t="s">
+        <v>8</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D134">
+        <v>64</v>
+      </c>
+      <c r="E134">
+        <v>45000</v>
+      </c>
+      <c r="F134">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A135" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B135" t="s">
+        <v>9</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D135">
+        <v>61</v>
+      </c>
+      <c r="E135">
+        <v>50000</v>
+      </c>
+      <c r="F135">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A136" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B136" t="s">
+        <v>10</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D136">
+        <v>76</v>
+      </c>
+      <c r="E136">
+        <v>55000</v>
+      </c>
+      <c r="F136">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A137" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B137" t="s">
+        <v>11</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D137">
+        <v>77</v>
+      </c>
+      <c r="E137">
+        <v>60000</v>
+      </c>
+      <c r="F137">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A138" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B138" t="s">
+        <v>8</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D138">
+        <v>64</v>
+      </c>
+      <c r="E138">
+        <v>45000</v>
+      </c>
+      <c r="F138">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A139" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B139" t="s">
+        <v>9</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D139">
+        <v>61</v>
+      </c>
+      <c r="E139">
+        <v>50000</v>
+      </c>
+      <c r="F139">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A140" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B140" t="s">
+        <v>10</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D140">
+        <v>76</v>
+      </c>
+      <c r="E140">
+        <v>55000</v>
+      </c>
+      <c r="F140">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A141" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B141" t="s">
+        <v>11</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D141">
+        <v>77</v>
+      </c>
+      <c r="E141">
+        <v>60000</v>
+      </c>
+      <c r="F141">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A142" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B142" t="s">
+        <v>8</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D142">
+        <v>64</v>
+      </c>
+      <c r="E142">
+        <v>45000</v>
+      </c>
+      <c r="F142">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A143" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B143" t="s">
+        <v>9</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D143">
+        <v>61</v>
+      </c>
+      <c r="E143">
+        <v>50000</v>
+      </c>
+      <c r="F143">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A144" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B144" t="s">
+        <v>10</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D144">
+        <v>76</v>
+      </c>
+      <c r="E144">
+        <v>55000</v>
+      </c>
+      <c r="F144">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A145" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B145" t="s">
+        <v>11</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D145">
+        <v>77</v>
+      </c>
+      <c r="E145">
+        <v>60000</v>
+      </c>
+      <c r="F145">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A146" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B146" t="s">
+        <v>8</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D146">
+        <v>64</v>
+      </c>
+      <c r="E146">
+        <v>45000</v>
+      </c>
+      <c r="F146">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A147" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B147" t="s">
+        <v>9</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D147">
+        <v>61</v>
+      </c>
+      <c r="E147">
+        <v>50000</v>
+      </c>
+      <c r="F147">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A148" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B148" t="s">
+        <v>10</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D148">
+        <v>76</v>
+      </c>
+      <c r="E148">
+        <v>55000</v>
+      </c>
+      <c r="F148">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A149" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B149" t="s">
+        <v>11</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D149">
+        <v>77</v>
+      </c>
+      <c r="E149">
+        <v>60000</v>
+      </c>
+      <c r="F149">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A150" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B150" t="b">
+        <v>0</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D150">
+        <v>64</v>
+      </c>
+      <c r="E150">
+        <v>45000</v>
+      </c>
+      <c r="F150">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A151" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B151" t="s">
+        <v>9</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D151">
+        <v>61</v>
+      </c>
+      <c r="E151">
+        <v>50000</v>
+      </c>
+      <c r="F151">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A152" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B152" t="s">
+        <v>10</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D152">
+        <v>76</v>
+      </c>
+      <c r="E152">
+        <v>55000</v>
+      </c>
+      <c r="F152">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A153" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B153" t="s">
+        <v>11</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D153">
+        <v>77</v>
+      </c>
+      <c r="E153">
+        <v>60000</v>
+      </c>
+      <c r="F153">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A154" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B154" t="s">
+        <v>8</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D154">
+        <v>64</v>
+      </c>
+      <c r="E154">
+        <v>45000</v>
+      </c>
+      <c r="F154">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A155" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B155" t="s">
+        <v>9</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D155">
+        <v>61</v>
+      </c>
+      <c r="E155">
+        <v>50000</v>
+      </c>
+      <c r="F155">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A156" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B156" t="s">
+        <v>10</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D156">
+        <v>76</v>
+      </c>
+      <c r="E156">
+        <v>55000</v>
+      </c>
+      <c r="F156">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A157" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B157" t="s">
+        <v>11</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D157">
+        <v>77</v>
+      </c>
+      <c r="E157">
+        <v>60000</v>
+      </c>
+      <c r="F157">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A158" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B158" t="s">
+        <v>8</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D158">
+        <v>64</v>
+      </c>
+      <c r="E158">
+        <v>45000</v>
+      </c>
+      <c r="F158">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A159" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B159" t="s">
+        <v>9</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D159">
+        <v>61</v>
+      </c>
+      <c r="E159">
+        <v>50000</v>
+      </c>
+      <c r="F159">
         <v>180</v>
       </c>
     </row>
@@ -3039,6 +3773,43 @@
     <hyperlink ref="A121" r:id="rId117" xr:uid="{59F0C557-64B0-2045-9226-0761F48DB1B4}"/>
     <hyperlink ref="A122" r:id="rId118" xr:uid="{189D99BE-4F95-D24E-B6B2-F3123876AC5E}"/>
     <hyperlink ref="A123" r:id="rId119" xr:uid="{34C8C161-8D39-6843-BDB3-F17DFCEFB540}"/>
+    <hyperlink ref="A2" r:id="rId120" xr:uid="{3BF1FDD7-8DAD-204D-8623-131CC7CA9867}"/>
+    <hyperlink ref="A124" r:id="rId121" xr:uid="{02B81AAF-F7A5-7744-851F-3028C34F5144}"/>
+    <hyperlink ref="A125" r:id="rId122" xr:uid="{CCAF7650-E04E-514E-97AF-5FE21FDB2261}"/>
+    <hyperlink ref="A126" r:id="rId123" xr:uid="{9EFED800-F77A-4140-8CA9-7F6C8E69D0B1}"/>
+    <hyperlink ref="A127" r:id="rId124" xr:uid="{F66384A0-B9B1-9C4B-B986-F902254464EC}"/>
+    <hyperlink ref="A128" r:id="rId125" xr:uid="{DAB82BA3-8C3B-BF43-AA05-BB49B3E6991B}"/>
+    <hyperlink ref="A129" r:id="rId126" xr:uid="{31EB9E8C-8010-8341-8A79-80E9CEED7CD8}"/>
+    <hyperlink ref="A130" r:id="rId127" xr:uid="{4B2A5ED6-CDD3-C34D-A4C3-F3FF6FCC7209}"/>
+    <hyperlink ref="A131" r:id="rId128" xr:uid="{38D4FF42-C4BE-2940-AAB8-11A125FAFDF4}"/>
+    <hyperlink ref="A132" r:id="rId129" xr:uid="{5C2F3EE3-8354-1047-AAED-31E294B5DE73}"/>
+    <hyperlink ref="A133" r:id="rId130" xr:uid="{755F963D-C7F4-2648-AB6F-FC4DC265C27E}"/>
+    <hyperlink ref="A134" r:id="rId131" xr:uid="{51E2560C-EF5D-954D-B3F0-3F81F212D0CB}"/>
+    <hyperlink ref="A135" r:id="rId132" xr:uid="{CD7458F2-FFD2-3A42-AEF8-38CCB9D0A94C}"/>
+    <hyperlink ref="A136" r:id="rId133" xr:uid="{B7ABB954-F954-494E-9C05-504DE73DFBE5}"/>
+    <hyperlink ref="A137" r:id="rId134" xr:uid="{0EA12938-6E53-644C-8FEB-5290FCD315E6}"/>
+    <hyperlink ref="A138" r:id="rId135" xr:uid="{B60FB548-A8C6-D647-9C6A-C2ED675C03FD}"/>
+    <hyperlink ref="A139" r:id="rId136" xr:uid="{EF6B3A55-9CC3-2A47-89B0-AEC5BA3D4C4A}"/>
+    <hyperlink ref="A140" r:id="rId137" xr:uid="{54EB7E8C-670E-9B4C-AC9C-17C88A9CF225}"/>
+    <hyperlink ref="A141" r:id="rId138" xr:uid="{5D5D5ED0-F465-534A-BC94-53D7F9B9D1FD}"/>
+    <hyperlink ref="A142" r:id="rId139" xr:uid="{DF5F2B67-95A5-C84F-912C-4A24F1F794B4}"/>
+    <hyperlink ref="A143" r:id="rId140" xr:uid="{591C76BC-D4B4-5243-ACF7-8FD15E6BD50C}"/>
+    <hyperlink ref="A144" r:id="rId141" xr:uid="{6287E02C-F02F-A047-8D0A-A6795B65273A}"/>
+    <hyperlink ref="A145" r:id="rId142" xr:uid="{7767A63E-ED80-CD43-BDB1-4B5C1481905F}"/>
+    <hyperlink ref="A146" r:id="rId143" xr:uid="{16FDA635-281E-AA4F-91DA-AB2C89BA3A77}"/>
+    <hyperlink ref="A147" r:id="rId144" xr:uid="{7474A533-F177-0B4D-81E9-2AE8438CA48D}"/>
+    <hyperlink ref="A148" r:id="rId145" xr:uid="{7F02A760-5ED0-3F46-9C93-34756D5ABD84}"/>
+    <hyperlink ref="A149" r:id="rId146" xr:uid="{93D90115-1192-2B43-97EA-282F5BC5E6B5}"/>
+    <hyperlink ref="A150" r:id="rId147" xr:uid="{A127E8FE-EC7D-1F40-8AA2-CBB49D275934}"/>
+    <hyperlink ref="A151" r:id="rId148" xr:uid="{D1AC58E3-6E6A-3F4D-9D80-E426869AE7FA}"/>
+    <hyperlink ref="A152" r:id="rId149" xr:uid="{512D3538-776F-2849-B040-F0379A1C523A}"/>
+    <hyperlink ref="A153" r:id="rId150" xr:uid="{F6360F22-5D4D-644B-8BBA-0E1B28FF2732}"/>
+    <hyperlink ref="A154" r:id="rId151" xr:uid="{8FDC0C0A-C535-3D4D-8B14-ACA1DC96282F}"/>
+    <hyperlink ref="A155" r:id="rId152" xr:uid="{8ED77AA0-D19A-C942-8A51-A2E8A70545D6}"/>
+    <hyperlink ref="A156" r:id="rId153" xr:uid="{243044ED-5350-E94C-8A0C-F995536EBF99}"/>
+    <hyperlink ref="A157" r:id="rId154" xr:uid="{FB5366DD-1A81-A949-8AF4-C89AC3EE00EC}"/>
+    <hyperlink ref="A158" r:id="rId155" xr:uid="{DA2F0CA5-F954-A040-8E53-BAFA3FB83DD5}"/>
+    <hyperlink ref="A159" r:id="rId156" xr:uid="{EDF1E6D2-30F0-F04C-A21F-E1D84F443187}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Issues Fixed, Kernel-PCA finished
</commit_message>
<xml_diff>
--- a/sampleDataSet.xlsx
+++ b/sampleDataSet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gilpasternak/Downloads/Likelihood/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC2BBBD-3D58-3E47-ADB4-566C733E060C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04551F16-08E0-D94C-B74A-609926555075}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16620" xr2:uid="{1F8DA360-E974-914A-BB29-6C10CB151BF2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="21">
   <si>
     <t>Email</t>
   </si>
@@ -95,10 +95,7 @@
     <t>Weight</t>
   </si>
   <si>
-    <t>ellen@gmail.com</t>
-  </si>
-  <si>
-    <t>Gil@syntheticData**</t>
+    <t>Gil@syntheticData*!@</t>
   </si>
 </sst>
 </file>
@@ -473,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22315E7-23A9-A543-A0A9-36943FB40866}">
   <dimension ref="A1:F159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="F134" sqref="F134"/>
+    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="99" workbookViewId="0">
+      <selection activeCell="A155" sqref="A155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -505,9 +502,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="A2" s="1"/>
       <c r="D2">
         <v>80</v>
       </c>
@@ -3116,8 +3111,8 @@
       <c r="A133" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B133" t="b">
-        <v>0</v>
+      <c r="B133" t="s">
+        <v>10</v>
       </c>
       <c r="C133" s="2" t="s">
         <v>15</v>
@@ -3456,8 +3451,8 @@
       <c r="A150" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B150" t="b">
-        <v>0</v>
+      <c r="B150" t="s">
+        <v>11</v>
       </c>
       <c r="C150" s="2" t="s">
         <v>15</v>
@@ -3574,7 +3569,7 @@
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B156" t="s">
         <v>10</v>
@@ -3773,43 +3768,42 @@
     <hyperlink ref="A121" r:id="rId117" xr:uid="{59F0C557-64B0-2045-9226-0761F48DB1B4}"/>
     <hyperlink ref="A122" r:id="rId118" xr:uid="{189D99BE-4F95-D24E-B6B2-F3123876AC5E}"/>
     <hyperlink ref="A123" r:id="rId119" xr:uid="{34C8C161-8D39-6843-BDB3-F17DFCEFB540}"/>
-    <hyperlink ref="A2" r:id="rId120" xr:uid="{3BF1FDD7-8DAD-204D-8623-131CC7CA9867}"/>
-    <hyperlink ref="A124" r:id="rId121" xr:uid="{02B81AAF-F7A5-7744-851F-3028C34F5144}"/>
-    <hyperlink ref="A125" r:id="rId122" xr:uid="{CCAF7650-E04E-514E-97AF-5FE21FDB2261}"/>
-    <hyperlink ref="A126" r:id="rId123" xr:uid="{9EFED800-F77A-4140-8CA9-7F6C8E69D0B1}"/>
-    <hyperlink ref="A127" r:id="rId124" xr:uid="{F66384A0-B9B1-9C4B-B986-F902254464EC}"/>
-    <hyperlink ref="A128" r:id="rId125" xr:uid="{DAB82BA3-8C3B-BF43-AA05-BB49B3E6991B}"/>
-    <hyperlink ref="A129" r:id="rId126" xr:uid="{31EB9E8C-8010-8341-8A79-80E9CEED7CD8}"/>
-    <hyperlink ref="A130" r:id="rId127" xr:uid="{4B2A5ED6-CDD3-C34D-A4C3-F3FF6FCC7209}"/>
-    <hyperlink ref="A131" r:id="rId128" xr:uid="{38D4FF42-C4BE-2940-AAB8-11A125FAFDF4}"/>
-    <hyperlink ref="A132" r:id="rId129" xr:uid="{5C2F3EE3-8354-1047-AAED-31E294B5DE73}"/>
-    <hyperlink ref="A133" r:id="rId130" xr:uid="{755F963D-C7F4-2648-AB6F-FC4DC265C27E}"/>
-    <hyperlink ref="A134" r:id="rId131" xr:uid="{51E2560C-EF5D-954D-B3F0-3F81F212D0CB}"/>
-    <hyperlink ref="A135" r:id="rId132" xr:uid="{CD7458F2-FFD2-3A42-AEF8-38CCB9D0A94C}"/>
-    <hyperlink ref="A136" r:id="rId133" xr:uid="{B7ABB954-F954-494E-9C05-504DE73DFBE5}"/>
-    <hyperlink ref="A137" r:id="rId134" xr:uid="{0EA12938-6E53-644C-8FEB-5290FCD315E6}"/>
-    <hyperlink ref="A138" r:id="rId135" xr:uid="{B60FB548-A8C6-D647-9C6A-C2ED675C03FD}"/>
-    <hyperlink ref="A139" r:id="rId136" xr:uid="{EF6B3A55-9CC3-2A47-89B0-AEC5BA3D4C4A}"/>
-    <hyperlink ref="A140" r:id="rId137" xr:uid="{54EB7E8C-670E-9B4C-AC9C-17C88A9CF225}"/>
-    <hyperlink ref="A141" r:id="rId138" xr:uid="{5D5D5ED0-F465-534A-BC94-53D7F9B9D1FD}"/>
-    <hyperlink ref="A142" r:id="rId139" xr:uid="{DF5F2B67-95A5-C84F-912C-4A24F1F794B4}"/>
-    <hyperlink ref="A143" r:id="rId140" xr:uid="{591C76BC-D4B4-5243-ACF7-8FD15E6BD50C}"/>
-    <hyperlink ref="A144" r:id="rId141" xr:uid="{6287E02C-F02F-A047-8D0A-A6795B65273A}"/>
-    <hyperlink ref="A145" r:id="rId142" xr:uid="{7767A63E-ED80-CD43-BDB1-4B5C1481905F}"/>
-    <hyperlink ref="A146" r:id="rId143" xr:uid="{16FDA635-281E-AA4F-91DA-AB2C89BA3A77}"/>
-    <hyperlink ref="A147" r:id="rId144" xr:uid="{7474A533-F177-0B4D-81E9-2AE8438CA48D}"/>
-    <hyperlink ref="A148" r:id="rId145" xr:uid="{7F02A760-5ED0-3F46-9C93-34756D5ABD84}"/>
-    <hyperlink ref="A149" r:id="rId146" xr:uid="{93D90115-1192-2B43-97EA-282F5BC5E6B5}"/>
-    <hyperlink ref="A150" r:id="rId147" xr:uid="{A127E8FE-EC7D-1F40-8AA2-CBB49D275934}"/>
-    <hyperlink ref="A151" r:id="rId148" xr:uid="{D1AC58E3-6E6A-3F4D-9D80-E426869AE7FA}"/>
-    <hyperlink ref="A152" r:id="rId149" xr:uid="{512D3538-776F-2849-B040-F0379A1C523A}"/>
-    <hyperlink ref="A153" r:id="rId150" xr:uid="{F6360F22-5D4D-644B-8BBA-0E1B28FF2732}"/>
-    <hyperlink ref="A154" r:id="rId151" xr:uid="{8FDC0C0A-C535-3D4D-8B14-ACA1DC96282F}"/>
-    <hyperlink ref="A155" r:id="rId152" xr:uid="{8ED77AA0-D19A-C942-8A51-A2E8A70545D6}"/>
-    <hyperlink ref="A156" r:id="rId153" xr:uid="{243044ED-5350-E94C-8A0C-F995536EBF99}"/>
-    <hyperlink ref="A157" r:id="rId154" xr:uid="{FB5366DD-1A81-A949-8AF4-C89AC3EE00EC}"/>
-    <hyperlink ref="A158" r:id="rId155" xr:uid="{DA2F0CA5-F954-A040-8E53-BAFA3FB83DD5}"/>
-    <hyperlink ref="A159" r:id="rId156" xr:uid="{EDF1E6D2-30F0-F04C-A21F-E1D84F443187}"/>
+    <hyperlink ref="A124" r:id="rId120" xr:uid="{02B81AAF-F7A5-7744-851F-3028C34F5144}"/>
+    <hyperlink ref="A125" r:id="rId121" xr:uid="{CCAF7650-E04E-514E-97AF-5FE21FDB2261}"/>
+    <hyperlink ref="A126" r:id="rId122" xr:uid="{9EFED800-F77A-4140-8CA9-7F6C8E69D0B1}"/>
+    <hyperlink ref="A127" r:id="rId123" xr:uid="{F66384A0-B9B1-9C4B-B986-F902254464EC}"/>
+    <hyperlink ref="A128" r:id="rId124" xr:uid="{DAB82BA3-8C3B-BF43-AA05-BB49B3E6991B}"/>
+    <hyperlink ref="A129" r:id="rId125" xr:uid="{31EB9E8C-8010-8341-8A79-80E9CEED7CD8}"/>
+    <hyperlink ref="A130" r:id="rId126" xr:uid="{4B2A5ED6-CDD3-C34D-A4C3-F3FF6FCC7209}"/>
+    <hyperlink ref="A131" r:id="rId127" xr:uid="{38D4FF42-C4BE-2940-AAB8-11A125FAFDF4}"/>
+    <hyperlink ref="A132" r:id="rId128" xr:uid="{5C2F3EE3-8354-1047-AAED-31E294B5DE73}"/>
+    <hyperlink ref="A133" r:id="rId129" xr:uid="{755F963D-C7F4-2648-AB6F-FC4DC265C27E}"/>
+    <hyperlink ref="A134" r:id="rId130" xr:uid="{51E2560C-EF5D-954D-B3F0-3F81F212D0CB}"/>
+    <hyperlink ref="A135" r:id="rId131" xr:uid="{CD7458F2-FFD2-3A42-AEF8-38CCB9D0A94C}"/>
+    <hyperlink ref="A136" r:id="rId132" xr:uid="{B7ABB954-F954-494E-9C05-504DE73DFBE5}"/>
+    <hyperlink ref="A137" r:id="rId133" xr:uid="{0EA12938-6E53-644C-8FEB-5290FCD315E6}"/>
+    <hyperlink ref="A138" r:id="rId134" xr:uid="{B60FB548-A8C6-D647-9C6A-C2ED675C03FD}"/>
+    <hyperlink ref="A139" r:id="rId135" xr:uid="{EF6B3A55-9CC3-2A47-89B0-AEC5BA3D4C4A}"/>
+    <hyperlink ref="A140" r:id="rId136" xr:uid="{54EB7E8C-670E-9B4C-AC9C-17C88A9CF225}"/>
+    <hyperlink ref="A141" r:id="rId137" xr:uid="{5D5D5ED0-F465-534A-BC94-53D7F9B9D1FD}"/>
+    <hyperlink ref="A142" r:id="rId138" xr:uid="{DF5F2B67-95A5-C84F-912C-4A24F1F794B4}"/>
+    <hyperlink ref="A143" r:id="rId139" xr:uid="{591C76BC-D4B4-5243-ACF7-8FD15E6BD50C}"/>
+    <hyperlink ref="A144" r:id="rId140" xr:uid="{6287E02C-F02F-A047-8D0A-A6795B65273A}"/>
+    <hyperlink ref="A145" r:id="rId141" xr:uid="{7767A63E-ED80-CD43-BDB1-4B5C1481905F}"/>
+    <hyperlink ref="A146" r:id="rId142" xr:uid="{16FDA635-281E-AA4F-91DA-AB2C89BA3A77}"/>
+    <hyperlink ref="A147" r:id="rId143" xr:uid="{7474A533-F177-0B4D-81E9-2AE8438CA48D}"/>
+    <hyperlink ref="A148" r:id="rId144" xr:uid="{7F02A760-5ED0-3F46-9C93-34756D5ABD84}"/>
+    <hyperlink ref="A149" r:id="rId145" xr:uid="{93D90115-1192-2B43-97EA-282F5BC5E6B5}"/>
+    <hyperlink ref="A150" r:id="rId146" xr:uid="{A127E8FE-EC7D-1F40-8AA2-CBB49D275934}"/>
+    <hyperlink ref="A151" r:id="rId147" xr:uid="{D1AC58E3-6E6A-3F4D-9D80-E426869AE7FA}"/>
+    <hyperlink ref="A152" r:id="rId148" xr:uid="{512D3538-776F-2849-B040-F0379A1C523A}"/>
+    <hyperlink ref="A153" r:id="rId149" xr:uid="{F6360F22-5D4D-644B-8BBA-0E1B28FF2732}"/>
+    <hyperlink ref="A154" r:id="rId150" xr:uid="{8FDC0C0A-C535-3D4D-8B14-ACA1DC96282F}"/>
+    <hyperlink ref="A155" r:id="rId151" xr:uid="{8ED77AA0-D19A-C942-8A51-A2E8A70545D6}"/>
+    <hyperlink ref="A156" r:id="rId152" xr:uid="{243044ED-5350-E94C-8A0C-F995536EBF99}"/>
+    <hyperlink ref="A157" r:id="rId153" xr:uid="{FB5366DD-1A81-A949-8AF4-C89AC3EE00EC}"/>
+    <hyperlink ref="A158" r:id="rId154" xr:uid="{DA2F0CA5-F954-A040-8E53-BAFA3FB83DD5}"/>
+    <hyperlink ref="A159" r:id="rId155" xr:uid="{EDF1E6D2-30F0-F04C-A21F-E1D84F443187}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>